<commit_message>
Information regaring inductor and diode added
</commit_message>
<xml_diff>
--- a/documents/Bost-Regler-Vergleich.xlsx
+++ b/documents/Bost-Regler-Vergleich.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_EinfacherLEDBlitzer\V2\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\diver_led_tools\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3666DA0-D9E6-4062-BBAA-AC29C4A8E5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C3BFD-9280-4B18-9688-656BF9380F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>Regler</t>
   </si>
@@ -173,6 +173,39 @@
   </si>
   <si>
     <t>I = U /R = 1,24 / 5100</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>WE-HEPC 33µH, 0,9A</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>B0540W</t>
+  </si>
+  <si>
+    <t>Strom prüfen!</t>
+  </si>
+  <si>
+    <t>710-74408063330</t>
+  </si>
+  <si>
+    <t>621-B054W-F</t>
+  </si>
+  <si>
+    <t>zu schwach, ideal wäre über 2A</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>kann nur 0,5A, ideal wäre auch hier &gt; 2A</t>
+  </si>
+  <si>
+    <t>946-MP3217DJLFZ</t>
   </si>
 </sst>
 </file>
@@ -182,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,8 +253,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +283,11 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -449,13 +494,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -498,31 +544,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="16" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Berechnung" xfId="3" builtinId="22"/>
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -544,15 +592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>31751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>183769</xdr:rowOff>
+      <xdr:rowOff>18263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -575,8 +623,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="406400" y="2825750"/>
-          <a:ext cx="4749800" cy="1961769"/>
+          <a:off x="355600" y="2794001"/>
+          <a:ext cx="4425950" cy="1828012"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -593,8 +641,8 @@
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>527760</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>267410</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>111509</xdr:rowOff>
     </xdr:to>
@@ -898,7 +946,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,32 +961,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="20" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="20" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="20" t="s">
+      <c r="N1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="22"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -1106,89 +1154,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EAC2F0-F4ED-4E07-9C09-BE7A68099197}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="23"/>
+    <col min="2" max="2" width="10.90625" style="20"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="39.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="22">
         <v>5</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="20">
         <v>1.24</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="25" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="26">
         <v>5100</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="28">
         <f>B3*(B1-B2)/B2</f>
         <v>15464.516129032258</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="30">
         <v>15000</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="28">
         <f>(B3+B5)*(B2/B3)</f>
         <v>4.8870588235294115</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K19" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>